<commit_message>
Additional input data updates to consolidate Cargo Type (#174)
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/BCbVT/Battery Cap by Veh Type.xlsx
+++ b/InputData/endo-learn/BCbVT/Battery Cap by Veh Type.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\endo-learn\BCbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\endo-learn\BCbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A931B0D-FFB1-49A1-B377-D593FBE3DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22635" windowHeight="10965"/>
+    <workbookView xWindow="7950" yWindow="405" windowWidth="25935" windowHeight="22050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="3" r:id="rId2"/>
-    <sheet name="BCbVT-passenger" sheetId="2" r:id="rId3"/>
-    <sheet name="BCbVT-freight" sheetId="4" r:id="rId4"/>
+    <sheet name="BCbVT" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>BCbVT Battery Capacity by Vehicle Type</t>
   </si>
@@ -149,24 +158,6 @@
     <t>https://en.wikipedia.org/wiki/Chevrolet_Volt</t>
   </si>
   <si>
-    <t>LDVs</t>
-  </si>
-  <si>
-    <t>HDVs</t>
-  </si>
-  <si>
-    <t>aircraft</t>
-  </si>
-  <si>
-    <t>rail</t>
-  </si>
-  <si>
-    <t>ships</t>
-  </si>
-  <si>
-    <t>motorbikes</t>
-  </si>
-  <si>
     <t>battery electric vehicle</t>
   </si>
   <si>
@@ -192,12 +183,48 @@
   </si>
   <si>
     <t>Battery Capacity (MW*hr/vehicle</t>
+  </si>
+  <si>
+    <t>passenger LDVs</t>
+  </si>
+  <si>
+    <t>passenger HDVs</t>
+  </si>
+  <si>
+    <t>passenger aircraft</t>
+  </si>
+  <si>
+    <t>passenger rail</t>
+  </si>
+  <si>
+    <t>passenger ships</t>
+  </si>
+  <si>
+    <t>passenger motorbikes</t>
+  </si>
+  <si>
+    <t>freight LDVs</t>
+  </si>
+  <si>
+    <t>freight HDVs</t>
+  </si>
+  <si>
+    <t>freight aircraft</t>
+  </si>
+  <si>
+    <t>freight rail</t>
+  </si>
+  <si>
+    <t>freight ships</t>
+  </si>
+  <si>
+    <t>freight motorbikes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -270,7 +297,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,23 +579,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="104.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -576,149 +603,149 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>2016</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>2018</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
-    <hyperlink ref="B21" r:id="rId3"/>
-    <hyperlink ref="B28" r:id="rId4"/>
-    <hyperlink ref="B33" r:id="rId5"/>
-    <hyperlink ref="B34" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B33" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B34" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -726,24 +753,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" customWidth="1"/>
-    <col min="2" max="2" width="28.265625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.7</v>
       </c>
@@ -751,7 +778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2/10^3</f>
         <v>6.9999999999999999E-4</v>
@@ -760,13 +787,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>75</v>
       </c>
@@ -774,7 +801,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>300</v>
       </c>
@@ -782,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>AVERAGE(A6:A7)</f>
         <v>187.5</v>
@@ -791,7 +818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A8/10^3</f>
         <v>0.1875</v>
@@ -800,13 +827,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>212</v>
       </c>
@@ -814,7 +841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A12/10^3</f>
         <v>0.21199999999999999</v>
@@ -823,13 +850,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -837,7 +864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>90</v>
       </c>
@@ -845,7 +872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -853,7 +880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <f>AVERAGE(A16:A18)</f>
         <v>73.333333333333329</v>
@@ -862,7 +889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f>A19/10^3</f>
         <v>7.3333333333333334E-2</v>
@@ -871,13 +898,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18.399999999999999</v>
       </c>
@@ -885,7 +912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8.8000000000000007</v>
       </c>
@@ -893,7 +920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>AVERAGE(A23:A24)</f>
         <v>13.6</v>
@@ -902,7 +929,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>A25/10^3</f>
         <v>1.3599999999999999E-2</v>
@@ -917,56 +944,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.59765625" customWidth="1"/>
-    <col min="2" max="5" width="18.59765625" customWidth="1"/>
-    <col min="6" max="6" width="22.59765625" customWidth="1"/>
-    <col min="7" max="7" width="18.1328125" customWidth="1"/>
-    <col min="8" max="8" width="19.86328125" customWidth="1"/>
-    <col min="9" max="9" width="18.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="B2" s="6">
         <f>Data!A20</f>
@@ -995,9 +1024,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <f>Data!A9</f>
@@ -1025,9 +1054,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1054,9 +1083,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1083,9 +1112,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1112,9 +1141,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <f>Data!A3</f>
@@ -1142,234 +1171,181 @@
         <v>0</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="15.265625" customWidth="1"/>
-    <col min="2" max="5" width="18.59765625" customWidth="1"/>
-    <col min="6" max="6" width="22.59765625" customWidth="1"/>
-    <col min="7" max="7" width="18.1328125" customWidth="1"/>
-    <col min="8" max="8" width="19.86328125" customWidth="1"/>
-    <col min="9" max="9" width="18.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="57" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="6">
         <f>Data!A20</f>
         <v>7.3333333333333334E-2</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <f>Data!A26</f>
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6">
         <f>Data!A13</f>
         <v>0.21199999999999999</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
         <f>Data!A3</f>
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>0</v>
       </c>
     </row>

</xml_diff>